<commit_message>
End of Today, added issues
</commit_message>
<xml_diff>
--- a/A01/Quality Req.xlsx
+++ b/A01/Quality Req.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>MIB must not be allowed to crash just because the tested system crashes</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Must support several kinds of different testing techniques</t>
   </si>
   <si>
-    <t>Impact</t>
-  </si>
-  <si>
     <t>Must run on any standard computer with the required performance</t>
   </si>
   <si>
@@ -49,27 +46,6 @@
   </si>
   <si>
     <t>Flexible validation rules for output</t>
-  </si>
-  <si>
-    <t>Changeablitity</t>
-  </si>
-  <si>
-    <t>Flexibility</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arbitrary number of input types      likely to happen once per costumer </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arbitrary number of output types      likely to happen once per costumer </t>
-  </si>
-  <si>
-    <t>Lower throughput</t>
-  </si>
-  <si>
-    <t>from standard computer to another computer type, not likely</t>
   </si>
   <si>
     <t>creating a log of all test data</t>
@@ -425,7 +401,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -440,16 +416,10 @@
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="E1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1"/>
@@ -458,93 +428,64 @@
       <c r="E2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="30">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E3" s="3"/>
       <c r="G3" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1">
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1">
       <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E9" s="2"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>5</v>
       </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+    </row>
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>